<commit_message>
-Optimización Libro Mayor -Se agregan cuentas contables en el reporte del libro mayor -Se termina el 14ter (Beta) -Se agrega exportación a Excel 14ter -Se modifican cuentas contables bases
</commit_message>
<xml_diff>
--- a/TryTestWeb/App_Data/EXCELMAYOR.xlsx
+++ b/TryTestWeb/App_Data/EXCELMAYOR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FACTURALABS\TryTestWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GEOGEST\TryTestWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27D3620-627D-4D98-B164-AFC1D2553445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA4CC79-F739-4338-BBDF-23855F5CF407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>FECHA</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>RAZONSOCIAL</t>
+  </si>
+  <si>
+    <t>CUENTA CONTABLE</t>
   </si>
 </sst>
 </file>
@@ -166,15 +169,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -187,6 +181,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H385"/>
+  <dimension ref="A1:I385"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,90 +483,91 @@
     <col min="3" max="3" width="54.7109375" customWidth="1"/>
     <col min="4" max="7" width="16.7109375" style="7" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="3"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -571,57 +575,61 @@
       <c r="D10"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="H16" s="1"/>

</xml_diff>

<commit_message>
-Se modifica reporte de libro mayor
</commit_message>
<xml_diff>
--- a/TryTestWeb/App_Data/EXCELMAYOR.xlsx
+++ b/TryTestWeb/App_Data/EXCELMAYOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GEOGEST\TryTestWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA4CC79-F739-4338-BBDF-23855F5CF407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C374A586-A071-45D6-A143-5223272E35F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,25 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>FECHA</t>
-  </si>
-  <si>
-    <t>COMPROBANTE</t>
-  </si>
-  <si>
-    <t>GLOSA</t>
-  </si>
-  <si>
-    <t>DEBE</t>
-  </si>
-  <si>
-    <t>HABER</t>
-  </si>
-  <si>
-    <t>SALDO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>LIBRO MAYOR DESDE "FECHAINICIO" A "FECHAFIN"</t>
   </si>
@@ -70,15 +52,6 @@
   </si>
   <si>
     <t>11916349-8</t>
-  </si>
-  <si>
-    <t>RUT</t>
-  </si>
-  <si>
-    <t>RAZONSOCIAL</t>
-  </si>
-  <si>
-    <t>CUENTA CONTABLE</t>
   </si>
 </sst>
 </file>
@@ -118,27 +91,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -169,18 +127,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -190,6 +136,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +431,7 @@
   <dimension ref="A1:I385"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,71 +445,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>8</v>
+      <c r="A1" s="11" t="s">
+        <v>2</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>9</v>
+      <c r="A2" s="11" t="s">
+        <v>3</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>10</v>
+      <c r="A3" s="13" t="s">
+        <v>4</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>11</v>
+      <c r="A4" s="13" t="s">
+        <v>5</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>12</v>
+      <c r="A5" s="11" t="s">
+        <v>6</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>13</v>
+      <c r="A6" s="11" t="s">
+        <v>7</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>14</v>
+      <c r="A7" s="12" t="s">
+        <v>8</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="3"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -559,18 +517,19 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="C8" s="5" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="D9"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D10"/>
       <c r="E10" s="10"/>
@@ -580,44 +539,26 @@
       <c r="D11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>

</xml_diff>